<commit_message>
change seconds to km
</commit_message>
<xml_diff>
--- a/data/inter_iit_data/clean_data_bangalore_pickups.xlsx
+++ b/data/inter_iit_data/clean_data_bangalore_pickups.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +436,7 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Unnamed: 0</t>
+          <t>id</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -461,10 +461,35 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>EDD</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>type</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>completed</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>itemID</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>routeId</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
           <t>latitude</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="M1" s="1" t="inlineStr">
         <is>
           <t>longitude</t>
         </is>
@@ -475,31 +500,42 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>1</v>
+        <v>2380</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1260, SY 35/4, SJR Tower's, 7th Phase, 24th Main Puttanhalli, JP Nagar, Bangalore</t>
+          <t>3rd Cross, 2nd Stage, Domlur, Bangalore</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>40834506264</v>
+        <v>123456789</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Leah West</t>
+          <t>Samay Raina2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>SKU_8</t>
-        </is>
-      </c>
-      <c r="G2" t="n">
-        <v>12.9156577</v>
-      </c>
-      <c r="H2" t="n">
-        <v>77.5994159</v>
+          <t>SKU_new0</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I2" t="b">
+        <v>0</v>
+      </c>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="n">
+        <v>12.9611795</v>
+      </c>
+      <c r="M2" t="n">
+        <v>77.5796242</v>
       </c>
     </row>
     <row r="3">
@@ -507,31 +543,42 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>2</v>
+        <v>2143</v>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>82/3, Third Floor, Khata 866, Panathur Main Road, Bhoganahalli Cross, Marathahalli, Bangalore</t>
+          <t>1260, SY 35/4, SJR Tower's, 7th Phase, 24th Main Puttanhalli, JP Nagar, Bangalore</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>81893229584</v>
+        <v>40834506264</v>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Ruben Thompson</t>
+          <t>Leah West</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>SKU_90</t>
-        </is>
-      </c>
-      <c r="G3" t="n">
-        <v>12.9365238</v>
-      </c>
-      <c r="H3" t="n">
-        <v>77.703783</v>
+          <t>SKU_8</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I3" t="b">
+        <v>0</v>
+      </c>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="n">
+        <v>12.9156577</v>
+      </c>
+      <c r="M3" t="n">
+        <v>77.5994159</v>
       </c>
     </row>
     <row r="4">
@@ -539,31 +586,42 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>3</v>
+        <v>2144</v>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Embassy Tech Square Food Court, Cessna Tech Park, Outer Ring Road, Kadubeesanahalli, Marathahalli, Bangalore</t>
+          <t>82/3, Third Floor, Khata 866, Panathur Main Road, Bhoganahalli Cross, Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>59723146139</v>
+        <v>81893229584</v>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Melva Little</t>
+          <t>Ruben Thompson</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>SKU_86</t>
-        </is>
-      </c>
-      <c r="G4" t="n">
-        <v>12.9360704</v>
-      </c>
-      <c r="H4" t="n">
-        <v>77.6935663</v>
+          <t>SKU_90</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I4" t="b">
+        <v>0</v>
+      </c>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="n">
+        <v>12.9365238</v>
+      </c>
+      <c r="M4" t="n">
+        <v>77.703783</v>
       </c>
     </row>
     <row r="5">
@@ -571,31 +629,42 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>4</v>
+        <v>2145</v>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>44, 3rd Cross, Marenahalli, 2nd Phase, JP Nagar, Bangalore</t>
+          <t>Embassy Tech Square Food Court, Cessna Tech Park, Outer Ring Road, Kadubeesanahalli, Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>13550952423</v>
+        <v>59723146139</v>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Mary Kirk</t>
+          <t>Melva Little</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>SKU_129</t>
-        </is>
-      </c>
-      <c r="G5" t="n">
-        <v>12.9135927</v>
-      </c>
-      <c r="H5" t="n">
-        <v>77.5873919</v>
+          <t>SKU_86</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="n">
+        <v>12.9360704</v>
+      </c>
+      <c r="M5" t="n">
+        <v>77.6935663</v>
       </c>
     </row>
     <row r="6">
@@ -603,31 +672,42 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>2146</v>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>2617, 27th Main, Sector 1, Opposite CPWD Complex, HSR, Bangalore</t>
+          <t>44, 3rd Cross, Marenahalli, 2nd Phase, JP Nagar, Bangalore</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>37256804721</v>
+        <v>13550952423</v>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Johnny Blake</t>
+          <t>Mary Kirk</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>SKU_29</t>
-        </is>
-      </c>
-      <c r="G6" t="n">
-        <v>12.9137071</v>
-      </c>
-      <c r="H6" t="n">
-        <v>77.651623</v>
+          <t>SKU_129</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="n">
+        <v>12.9135927</v>
+      </c>
+      <c r="M6" t="n">
+        <v>77.5873919</v>
       </c>
     </row>
     <row r="7">
@@ -635,31 +715,42 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>6</v>
+        <v>2147</v>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>493, 13th Cross, 2nd Stage, Behind BDA Complex, Indiranagar, Bangalore</t>
+          <t>2617, 27th Main, Sector 1, Opposite CPWD Complex, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>98320322280</v>
+        <v>37256804721</v>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Kathryn Zuhlke</t>
+          <t>Johnny Blake</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>SKU_103</t>
-        </is>
-      </c>
-      <c r="G7" t="n">
-        <v>12.9773122</v>
-      </c>
-      <c r="H7" t="n">
-        <v>77.635937</v>
+          <t>SKU_29</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I7" t="b">
+        <v>0</v>
+      </c>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="n">
+        <v>12.9137071</v>
+      </c>
+      <c r="M7" t="n">
+        <v>77.651623</v>
       </c>
     </row>
     <row r="8">
@@ -667,31 +758,42 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>7</v>
+        <v>2148</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>2334, Aarush Arcade, 17th Cross, 1st Sector, HSR, Bangalore</t>
+          <t>493, 13th Cross, 2nd Stage, Behind BDA Complex, Indiranagar, Bangalore</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>64727690316</v>
+        <v>98320322280</v>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Charles Shelley</t>
+          <t>Kathryn Zuhlke</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>SKU_79</t>
-        </is>
-      </c>
-      <c r="G8" t="n">
-        <v>12.9122542</v>
-      </c>
-      <c r="H8" t="n">
-        <v>77.63633109999999</v>
+          <t>SKU_103</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr"/>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="n">
+        <v>12.9773122</v>
+      </c>
+      <c r="M8" t="n">
+        <v>77.635937</v>
       </c>
     </row>
     <row r="9">
@@ -699,31 +801,42 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>2149</v>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>1659, 27th Main Road, Sector 2, HSR Layout, HSR, Bangalore</t>
+          <t>2334, Aarush Arcade, 17th Cross, 1st Sector, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>33739970099</v>
+        <v>64727690316</v>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Monica Troxler</t>
+          <t>Charles Shelley</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>SKU_39</t>
-        </is>
-      </c>
-      <c r="G9" t="n">
-        <v>12.9099715</v>
-      </c>
-      <c r="H9" t="n">
-        <v>77.6518782</v>
+          <t>SKU_79</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr"/>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I9" t="b">
+        <v>0</v>
+      </c>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="n">
+        <v>12.9122542</v>
+      </c>
+      <c r="M9" t="n">
+        <v>77.63633109999999</v>
       </c>
     </row>
     <row r="10">
@@ -731,31 +844,42 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>9</v>
+        <v>2150</v>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>31st Main, Near NIFT, Sector 1, HSR, Bangalore</t>
+          <t>1659, 27th Main Road, Sector 2, HSR Layout, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>70719650178</v>
+        <v>33739970099</v>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Barbara Baumberger</t>
+          <t>Monica Troxler</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>SKU_118</t>
-        </is>
-      </c>
-      <c r="G10" t="n">
-        <v>12.9114016</v>
-      </c>
-      <c r="H10" t="n">
-        <v>77.6535232</v>
+          <t>SKU_39</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr"/>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I10" t="b">
+        <v>0</v>
+      </c>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="n">
+        <v>12.9099715</v>
+      </c>
+      <c r="M10" t="n">
+        <v>77.6518782</v>
       </c>
     </row>
     <row r="11">
@@ -763,31 +887,42 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>10</v>
+        <v>2151</v>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>19/4 &amp; 27, Ground Floor, Indiqube Alpha, Panathur Junction, Kadubisanahalli, Sarjapur Outer Ring Road, Marathahalli, Bangalore</t>
+          <t>31st Main, Near NIFT, Sector 1, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>33192159992</v>
+        <v>70719650178</v>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>Judy Epson</t>
+          <t>Barbara Baumberger</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>SKU_43</t>
-        </is>
-      </c>
-      <c r="G11" t="n">
-        <v>12.9399931</v>
-      </c>
-      <c r="H11" t="n">
-        <v>77.6962218</v>
+          <t>SKU_118</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr"/>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I11" t="b">
+        <v>0</v>
+      </c>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="n">
+        <v>12.9114016</v>
+      </c>
+      <c r="M11" t="n">
+        <v>77.6535232</v>
       </c>
     </row>
     <row r="12">
@@ -795,31 +930,42 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>11</v>
+        <v>2152</v>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>322, Shalini Complex, CMH Road, Indiranagar, Bangalore</t>
+          <t>19/4 &amp; 27, Ground Floor, Indiqube Alpha, Panathur Junction, Kadubisanahalli, Sarjapur Outer Ring Road, Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>87348538617</v>
+        <v>33192159992</v>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Albert Rosol</t>
+          <t>Judy Epson</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>SKU_28</t>
-        </is>
-      </c>
-      <c r="G12" t="n">
-        <v>12.9783143</v>
-      </c>
-      <c r="H12" t="n">
-        <v>77.637585</v>
+          <t>SKU_43</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I12" t="b">
+        <v>0</v>
+      </c>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
+        <v>12.9399931</v>
+      </c>
+      <c r="M12" t="n">
+        <v>77.6962218</v>
       </c>
     </row>
     <row r="13">
@@ -827,31 +973,42 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>12</v>
+        <v>2153</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Ground Floor, Figure and Fitness Gym, ESI Hospital Road, Double Road, Stage 3, Indiranagar, Bangalore</t>
+          <t>322, Shalini Complex, CMH Road, Indiranagar, Bangalore</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>90135330114</v>
+        <v>87348538617</v>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Raymond May</t>
+          <t>Albert Rosol</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>SKU_131</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>12.9711854</v>
-      </c>
-      <c r="H13" t="n">
-        <v>77.63690989999999</v>
+          <t>SKU_28</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I13" t="b">
+        <v>0</v>
+      </c>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="n">
+        <v>12.9783143</v>
+      </c>
+      <c r="M13" t="n">
+        <v>77.637585</v>
       </c>
     </row>
     <row r="14">
@@ -859,31 +1016,42 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>13</v>
+        <v>2154</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>844, Binnamangala, 1st Stage, Near B.D.A Complex, Double Road, Indiranagar, Bangalore</t>
+          <t>Ground Floor, Figure and Fitness Gym, ESI Hospital Road, Double Road, Stage 3, Indiranagar, Bangalore</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>98618659069</v>
+        <v>90135330114</v>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Robert Davis</t>
+          <t>Raymond May</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>SKU_43</t>
-        </is>
-      </c>
-      <c r="G14" t="n">
-        <v>12.9821969</v>
-      </c>
-      <c r="H14" t="n">
-        <v>77.63688719999999</v>
+          <t>SKU_131</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr"/>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I14" t="b">
+        <v>0</v>
+      </c>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="n">
+        <v>12.9711854</v>
+      </c>
+      <c r="M14" t="n">
+        <v>77.63690989999999</v>
       </c>
     </row>
     <row r="15">
@@ -891,31 +1059,42 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>14</v>
+        <v>2155</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>3rd Cross, 2nd Stage, Domlur, Bangalore</t>
+          <t>844, Binnamangala, 1st Stage, Near B.D.A Complex, Double Road, Indiranagar, Bangalore</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>37317986613</v>
+        <v>98618659069</v>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Karen Turner</t>
+          <t>Robert Davis</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>SKU_106</t>
-        </is>
-      </c>
-      <c r="G15" t="n">
-        <v>12.9611795</v>
-      </c>
-      <c r="H15" t="n">
-        <v>77.5796242</v>
+          <t>SKU_43</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr"/>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I15" t="b">
+        <v>0</v>
+      </c>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="n">
+        <v>12.9821969</v>
+      </c>
+      <c r="M15" t="n">
+        <v>77.63688719999999</v>
       </c>
     </row>
     <row r="16">
@@ -923,31 +1102,42 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>15</v>
+        <v>2156</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Shop 217, 2nd Main Road, Kadubeesanahalli Croma, Back Side Road, Near Kumbeshwara Temple Marathahalli, Bangalore</t>
+          <t>3rd Cross, 2nd Stage, Domlur, Bangalore</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>83760820881</v>
+        <v>37317986613</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Morris Delacruz</t>
+          <t>Karen Turner</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>SKU_33</t>
-        </is>
-      </c>
-      <c r="G16" t="n">
-        <v>12.973296</v>
-      </c>
-      <c r="H16" t="n">
-        <v>77.6957888</v>
+          <t>SKU_106</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr"/>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I16" t="b">
+        <v>0</v>
+      </c>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="n">
+        <v>12.9611795</v>
+      </c>
+      <c r="M16" t="n">
+        <v>77.5796242</v>
       </c>
     </row>
     <row r="17">
@@ -955,31 +1145,42 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>16</v>
+        <v>2157</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>68, Appareddy Palya, Near ESI Hospital, HAL 2nd Stage, Double Road, Indiranagar, Bangalore</t>
+          <t>Shop 217, 2nd Main Road, Kadubeesanahalli Croma, Back Side Road, Near Kumbeshwara Temple Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D17" t="n">
-        <v>19222028019</v>
+        <v>83760820881</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Russell Repp</t>
+          <t>Morris Delacruz</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>SKU_47</t>
-        </is>
-      </c>
-      <c r="G17" t="n">
-        <v>12.9728579</v>
-      </c>
-      <c r="H17" t="n">
-        <v>77.63695440000001</v>
+          <t>SKU_33</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr"/>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I17" t="b">
+        <v>0</v>
+      </c>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="n">
+        <v>12.973296</v>
+      </c>
+      <c r="M17" t="n">
+        <v>77.6957888</v>
       </c>
     </row>
     <row r="18">
@@ -987,31 +1188,42 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>17</v>
+        <v>2158</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>89/1, Monnekollal Village, Varthur Hobli, Outer Ring Road, Marathahalli, Bangalore</t>
+          <t>68, Appareddy Palya, Near ESI Hospital, HAL 2nd Stage, Double Road, Indiranagar, Bangalore</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>35278429230</v>
+        <v>19222028019</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Anna Parsons</t>
+          <t>Russell Repp</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>SKU_11</t>
-        </is>
-      </c>
-      <c r="G18" t="n">
-        <v>12.9577656</v>
-      </c>
-      <c r="H18" t="n">
-        <v>77.70117089999999</v>
+          <t>SKU_47</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr"/>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I18" t="b">
+        <v>0</v>
+      </c>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="n">
+        <v>12.9728579</v>
+      </c>
+      <c r="M18" t="n">
+        <v>77.63695440000001</v>
       </c>
     </row>
     <row r="19">
@@ -1019,31 +1231,42 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>18</v>
+        <v>2159</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Outer Ring Road, Opposite to JP Morgan, Kodbisanhalli, Marathahalli, Bangalore</t>
+          <t>89/1, Monnekollal Village, Varthur Hobli, Outer Ring Road, Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>85641566876</v>
+        <v>35278429230</v>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Antwan Howell</t>
+          <t>Anna Parsons</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>SKU_65</t>
-        </is>
-      </c>
-      <c r="G19" t="n">
-        <v>12.9428771</v>
-      </c>
-      <c r="H19" t="n">
-        <v>77.6966127</v>
+          <t>SKU_11</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr"/>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I19" t="b">
+        <v>0</v>
+      </c>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="n">
+        <v>12.9577656</v>
+      </c>
+      <c r="M19" t="n">
+        <v>77.70117089999999</v>
       </c>
     </row>
     <row r="20">
@@ -1051,31 +1274,42 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>19</v>
+        <v>2160</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>2318, Sector 1, Near NIFT College, HSR, Bangalore</t>
+          <t>Outer Ring Road, Opposite to JP Morgan, Kodbisanhalli, Marathahalli, Bangalore</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>44350146864</v>
+        <v>85641566876</v>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Ruth Donaldson</t>
+          <t>Antwan Howell</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>SKU_80</t>
-        </is>
-      </c>
-      <c r="G20" t="n">
-        <v>12.9175337</v>
-      </c>
-      <c r="H20" t="n">
-        <v>77.65045719999999</v>
+          <t>SKU_65</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr"/>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I20" t="b">
+        <v>0</v>
+      </c>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="n">
+        <v>12.9428771</v>
+      </c>
+      <c r="M20" t="n">
+        <v>77.6966127</v>
       </c>
     </row>
     <row r="21">
@@ -1083,31 +1317,42 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>20</v>
+        <v>2161</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>697, 12th Cross, 27th Main, 1st Sector, HSR, Bangalore</t>
+          <t>2318, Sector 1, Near NIFT College, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>35688482050</v>
+        <v>44350146864</v>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Cecilia Henderson</t>
+          <t>Ruth Donaldson</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>SKU_88</t>
-        </is>
-      </c>
-      <c r="G21" t="n">
-        <v>12.916185</v>
-      </c>
-      <c r="H21" t="n">
-        <v>77.65142400000001</v>
+          <t>SKU_80</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr"/>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I21" t="b">
+        <v>0</v>
+      </c>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="n">
+        <v>12.9175337</v>
+      </c>
+      <c r="M21" t="n">
+        <v>77.65045719999999</v>
       </c>
     </row>
     <row r="22">
@@ -1115,31 +1360,42 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>21</v>
+        <v>2162</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>1260 SY 35/4 SJR Tower's, 24th Main Puttanhalli, JP Nagar 7th Phase, Bangalore</t>
+          <t>697, 12th Cross, 27th Main, 1st Sector, HSR, Bangalore</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>75730852176</v>
+        <v>35688482050</v>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Jonathan Nelson</t>
+          <t>Cecilia Henderson</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>SKU_103</t>
-        </is>
-      </c>
-      <c r="G22" t="n">
-        <v>12.9003937</v>
-      </c>
-      <c r="H22" t="n">
-        <v>77.5858415</v>
+          <t>SKU_88</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr"/>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I22" t="b">
+        <v>0</v>
+      </c>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="n">
+        <v>12.916185</v>
+      </c>
+      <c r="M22" t="n">
+        <v>77.65142400000001</v>
       </c>
     </row>
     <row r="23">
@@ -1147,30 +1403,84 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>23</v>
+        <v>2163</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
+          <t>1260 SY 35/4 SJR Tower's, 24th Main Puttanhalli, JP Nagar 7th Phase, Bangalore</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
+        <v>75730852176</v>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>Jonathan Nelson</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>SKU_103</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr"/>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I23" t="b">
+        <v>0</v>
+      </c>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="n">
+        <v>12.9003937</v>
+      </c>
+      <c r="M23" t="n">
+        <v>77.5858415</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="1" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="n">
+        <v>2164</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
           <t>915, 24th Main Road, 2nd Phase, Mayura Circle, JP Nagar, Bangalore</t>
         </is>
       </c>
-      <c r="D23" t="n">
+      <c r="D24" t="n">
         <v>65256560203</v>
       </c>
-      <c r="E23" t="inlineStr">
+      <c r="E24" t="inlineStr">
         <is>
           <t>David Finn</t>
         </is>
       </c>
-      <c r="F23" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>SKU_148</t>
         </is>
       </c>
-      <c r="G23" t="n">
+      <c r="G24" t="inlineStr"/>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Pickup</t>
+        </is>
+      </c>
+      <c r="I24" t="b">
+        <v>0</v>
+      </c>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="n">
         <v>12.9102386</v>
       </c>
-      <c r="H23" t="n">
+      <c r="M24" t="n">
         <v>77.58589619999999</v>
       </c>
     </row>

</xml_diff>